<commit_message>
20170906T010 - EO completed.
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPDResponse-CriteriaTaxonomy-REGULATED-V02.00.00.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPDResponse-CriteriaTaxonomy-REGULATED-V02.00.00.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="8400"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="20730" windowHeight="8400" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="OTHER-EO-SHELTERED" sheetId="25" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="79">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -241,16 +241,22 @@
     <t>CRITERION.OTHER.EO_DATA.SUBCONTRACTS_WITH_THIRD_PARTIES</t>
   </si>
   <si>
-    <t>d5fe5a71-7fd3-4910-b6f4-5cd2a4d23524</t>
-  </si>
-  <si>
-    <t>[Proposed subcontractors]</t>
-  </si>
-  <si>
-    <t>7f18c64e-ae09-4646-9400-f3666d50af51</t>
-  </si>
-  <si>
-    <t>If yes and in so far as known, please list the proposed subcontractors</t>
+    <t>0..n</t>
+  </si>
+  <si>
+    <t>979fc579-d3d7-444b-861f-f7ac31c4f666</t>
+  </si>
+  <si>
+    <t>Name of the entity</t>
+  </si>
+  <si>
+    <t>ID of the entity</t>
+  </si>
+  <si>
+    <t>IDENTIFIER</t>
+  </si>
+  <si>
+    <t>Activity of the entity (for this specific procedure)</t>
   </si>
 </sst>
 </file>
@@ -621,7 +627,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -736,6 +742,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -782,7 +803,7 @@
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -874,17 +895,14 @@
     <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1231,7 +1249,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1604,7 +1624,7 @@
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="21"/>
-      <c r="S7" t="s">
+      <c r="S7" s="5" t="s">
         <v>33</v>
       </c>
       <c r="T7" s="23" t="s">
@@ -4670,7 +4690,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z137"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5860,893 +5882,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y131"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="10" style="11" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="1.85546875" style="11" customWidth="1"/>
-    <col min="10" max="11" width="2.7109375" style="11" customWidth="1"/>
-    <col min="12" max="16" width="2.7109375" style="11" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" style="11" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="11" customWidth="1"/>
-    <col min="19" max="20" width="11.42578125" style="11"/>
-    <col min="21" max="21" width="11.42578125" style="16"/>
-    <col min="22" max="23" width="11.42578125" style="11"/>
-    <col min="24" max="24" width="11.42578125" style="16"/>
-    <col min="25" max="16384" width="11.42578125" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3">
-        <v>1</v>
-      </c>
-      <c r="B1" s="4">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4">
-        <v>4</v>
-      </c>
-      <c r="E1" s="3">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4">
-        <v>6</v>
-      </c>
-      <c r="G1" s="3">
-        <v>7</v>
-      </c>
-      <c r="H1" s="4">
-        <v>8</v>
-      </c>
-      <c r="I1" s="3">
-        <v>9</v>
-      </c>
-      <c r="J1" s="4">
-        <v>10</v>
-      </c>
-      <c r="K1" s="3">
-        <v>11</v>
-      </c>
-      <c r="L1" s="4">
-        <v>12</v>
-      </c>
-      <c r="M1" s="3">
-        <v>13</v>
-      </c>
-      <c r="N1" s="4">
-        <v>14</v>
-      </c>
-      <c r="O1" s="3">
-        <v>15</v>
-      </c>
-      <c r="P1" s="4">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="3">
-        <v>17</v>
-      </c>
-      <c r="R1" s="4">
-        <v>18</v>
-      </c>
-      <c r="S1" s="3">
-        <v>19</v>
-      </c>
-      <c r="T1" s="4">
-        <v>20</v>
-      </c>
-      <c r="U1" s="13">
-        <v>21</v>
-      </c>
-      <c r="V1" s="4">
-        <v>22</v>
-      </c>
-      <c r="W1" s="3">
-        <v>23</v>
-      </c>
-      <c r="X1" s="14">
-        <v>24</v>
-      </c>
-      <c r="Y1" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>62</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="S3" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="T3" s="8"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="X3" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y3" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="U4" s="18">
-        <v>1</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="W4" t="s">
-        <v>55</v>
-      </c>
-      <c r="X4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y4" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="U5" s="18">
-        <v>1</v>
-      </c>
-      <c r="V5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="W5" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="X5" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="19"/>
-    </row>
-    <row r="7" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="S7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="T7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="U7" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="V7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="W7" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="X7" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="X8" s="11"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="X9" s="11"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="X10" s="11"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="X11" s="11"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="X12" s="11"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="X13" s="11"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="X14" s="11"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="X15" s="11"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="X16" s="11"/>
-    </row>
-    <row r="17" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U17" s="11"/>
-      <c r="X17" s="11"/>
-    </row>
-    <row r="18" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U18" s="11"/>
-      <c r="X18" s="11"/>
-    </row>
-    <row r="19" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U19" s="11"/>
-      <c r="X19" s="11"/>
-    </row>
-    <row r="20" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U20" s="11"/>
-      <c r="X20" s="11"/>
-    </row>
-    <row r="21" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U21" s="11"/>
-      <c r="X21" s="11"/>
-    </row>
-    <row r="22" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U22" s="11"/>
-      <c r="X22" s="11"/>
-    </row>
-    <row r="23" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U23" s="11"/>
-      <c r="X23" s="11"/>
-    </row>
-    <row r="24" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U24" s="11"/>
-      <c r="X24" s="11"/>
-    </row>
-    <row r="25" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U25" s="11"/>
-      <c r="X25" s="11"/>
-    </row>
-    <row r="26" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U26" s="11"/>
-      <c r="X26" s="11"/>
-    </row>
-    <row r="27" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U27" s="11"/>
-      <c r="X27" s="11"/>
-    </row>
-    <row r="28" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U28" s="11"/>
-      <c r="X28" s="11"/>
-    </row>
-    <row r="29" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U29" s="11"/>
-      <c r="X29" s="11"/>
-    </row>
-    <row r="30" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U30" s="11"/>
-      <c r="X30" s="11"/>
-    </row>
-    <row r="31" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U31" s="11"/>
-      <c r="X31" s="11"/>
-    </row>
-    <row r="32" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U32" s="11"/>
-      <c r="X32" s="11"/>
-    </row>
-    <row r="33" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U33" s="11"/>
-      <c r="X33" s="11"/>
-    </row>
-    <row r="34" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U34" s="11"/>
-      <c r="X34" s="11"/>
-    </row>
-    <row r="35" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U35" s="11"/>
-      <c r="X35" s="11"/>
-    </row>
-    <row r="36" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U36" s="11"/>
-      <c r="X36" s="11"/>
-    </row>
-    <row r="37" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U37" s="11"/>
-      <c r="X37" s="11"/>
-    </row>
-    <row r="38" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U38" s="11"/>
-      <c r="X38" s="11"/>
-    </row>
-    <row r="39" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U39" s="11"/>
-      <c r="X39" s="11"/>
-    </row>
-    <row r="40" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U40" s="11"/>
-      <c r="X40" s="11"/>
-    </row>
-    <row r="41" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U41" s="11"/>
-      <c r="X41" s="11"/>
-    </row>
-    <row r="42" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U42" s="11"/>
-      <c r="X42" s="11"/>
-    </row>
-    <row r="43" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U43" s="11"/>
-      <c r="X43" s="11"/>
-    </row>
-    <row r="44" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U44" s="11"/>
-      <c r="X44" s="11"/>
-    </row>
-    <row r="45" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U45" s="11"/>
-      <c r="X45" s="11"/>
-    </row>
-    <row r="46" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U46" s="11"/>
-      <c r="X46" s="11"/>
-    </row>
-    <row r="47" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U47" s="11"/>
-      <c r="X47" s="11"/>
-    </row>
-    <row r="48" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U48" s="11"/>
-      <c r="X48" s="11"/>
-    </row>
-    <row r="49" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U49" s="11"/>
-      <c r="X49" s="11"/>
-    </row>
-    <row r="50" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U50" s="11"/>
-      <c r="X50" s="11"/>
-    </row>
-    <row r="51" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U51" s="11"/>
-      <c r="X51" s="11"/>
-    </row>
-    <row r="52" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U52" s="11"/>
-      <c r="X52" s="11"/>
-    </row>
-    <row r="53" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U53" s="11"/>
-      <c r="X53" s="11"/>
-    </row>
-    <row r="54" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U54" s="11"/>
-      <c r="X54" s="11"/>
-    </row>
-    <row r="55" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U55" s="11"/>
-      <c r="X55" s="11"/>
-    </row>
-    <row r="56" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U56" s="11"/>
-      <c r="X56" s="11"/>
-    </row>
-    <row r="57" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U57" s="11"/>
-      <c r="X57" s="11"/>
-    </row>
-    <row r="58" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U58" s="11"/>
-      <c r="X58" s="11"/>
-    </row>
-    <row r="59" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U59" s="11"/>
-      <c r="X59" s="11"/>
-    </row>
-    <row r="60" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U60" s="11"/>
-      <c r="X60" s="11"/>
-    </row>
-    <row r="61" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U61" s="11"/>
-      <c r="X61" s="11"/>
-    </row>
-    <row r="62" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U62" s="11"/>
-      <c r="X62" s="11"/>
-    </row>
-    <row r="63" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U63" s="11"/>
-      <c r="X63" s="11"/>
-    </row>
-    <row r="64" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U64" s="11"/>
-      <c r="X64" s="11"/>
-    </row>
-    <row r="65" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U65" s="11"/>
-      <c r="X65" s="11"/>
-    </row>
-    <row r="66" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U66" s="11"/>
-      <c r="X66" s="11"/>
-    </row>
-    <row r="67" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U67" s="11"/>
-      <c r="X67" s="11"/>
-    </row>
-    <row r="68" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U68" s="11"/>
-      <c r="X68" s="11"/>
-    </row>
-    <row r="69" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U69" s="11"/>
-      <c r="X69" s="11"/>
-    </row>
-    <row r="70" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U70" s="11"/>
-      <c r="X70" s="11"/>
-    </row>
-    <row r="71" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U71" s="11"/>
-      <c r="X71" s="11"/>
-    </row>
-    <row r="72" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U72" s="11"/>
-      <c r="X72" s="11"/>
-    </row>
-    <row r="73" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U73" s="11"/>
-      <c r="X73" s="11"/>
-    </row>
-    <row r="74" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U74" s="11"/>
-      <c r="X74" s="11"/>
-    </row>
-    <row r="75" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U75" s="11"/>
-      <c r="X75" s="11"/>
-    </row>
-    <row r="76" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U76" s="11"/>
-      <c r="X76" s="11"/>
-    </row>
-    <row r="77" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U77" s="11"/>
-      <c r="X77" s="11"/>
-    </row>
-    <row r="78" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U78" s="11"/>
-      <c r="X78" s="11"/>
-    </row>
-    <row r="79" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U79" s="11"/>
-      <c r="X79" s="11"/>
-    </row>
-    <row r="80" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U80" s="11"/>
-      <c r="X80" s="11"/>
-    </row>
-    <row r="81" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U81" s="11"/>
-      <c r="X81" s="11"/>
-    </row>
-    <row r="82" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U82" s="11"/>
-      <c r="X82" s="11"/>
-    </row>
-    <row r="83" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U83" s="11"/>
-      <c r="X83" s="11"/>
-    </row>
-    <row r="84" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U84" s="11"/>
-      <c r="X84" s="11"/>
-    </row>
-    <row r="85" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U85" s="11"/>
-      <c r="X85" s="11"/>
-    </row>
-    <row r="86" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U86" s="11"/>
-      <c r="X86" s="11"/>
-    </row>
-    <row r="87" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U87" s="11"/>
-      <c r="X87" s="11"/>
-    </row>
-    <row r="88" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U88" s="11"/>
-      <c r="X88" s="11"/>
-    </row>
-    <row r="89" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U89" s="11"/>
-      <c r="X89" s="11"/>
-    </row>
-    <row r="90" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U90" s="11"/>
-      <c r="X90" s="11"/>
-    </row>
-    <row r="91" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U91" s="11"/>
-      <c r="X91" s="11"/>
-    </row>
-    <row r="92" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U92" s="11"/>
-      <c r="X92" s="11"/>
-    </row>
-    <row r="93" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U93" s="11"/>
-      <c r="X93" s="11"/>
-    </row>
-    <row r="94" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U94" s="11"/>
-      <c r="X94" s="11"/>
-    </row>
-    <row r="95" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U95" s="11"/>
-      <c r="X95" s="11"/>
-    </row>
-    <row r="96" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U96" s="11"/>
-      <c r="X96" s="11"/>
-    </row>
-    <row r="97" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U97" s="11"/>
-      <c r="X97" s="11"/>
-    </row>
-    <row r="98" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U98" s="11"/>
-      <c r="X98" s="11"/>
-    </row>
-    <row r="99" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U99" s="11"/>
-      <c r="X99" s="11"/>
-    </row>
-    <row r="100" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U100" s="11"/>
-      <c r="X100" s="11"/>
-    </row>
-    <row r="101" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U101" s="11"/>
-      <c r="X101" s="11"/>
-    </row>
-    <row r="102" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U102" s="11"/>
-      <c r="X102" s="11"/>
-    </row>
-    <row r="103" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U103" s="11"/>
-      <c r="X103" s="11"/>
-    </row>
-    <row r="104" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U104" s="11"/>
-      <c r="X104" s="11"/>
-    </row>
-    <row r="105" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U105" s="11"/>
-      <c r="X105" s="11"/>
-    </row>
-    <row r="106" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U106" s="11"/>
-      <c r="X106" s="11"/>
-    </row>
-    <row r="107" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U107" s="11"/>
-      <c r="X107" s="11"/>
-    </row>
-    <row r="108" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U108" s="11"/>
-      <c r="X108" s="11"/>
-    </row>
-    <row r="109" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U109" s="11"/>
-      <c r="X109" s="11"/>
-    </row>
-    <row r="110" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U110" s="11"/>
-      <c r="X110" s="11"/>
-    </row>
-    <row r="111" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U111" s="11"/>
-      <c r="X111" s="11"/>
-    </row>
-    <row r="112" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U112" s="11"/>
-      <c r="X112" s="11"/>
-    </row>
-    <row r="113" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U113" s="11"/>
-      <c r="X113" s="11"/>
-    </row>
-    <row r="114" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U114" s="11"/>
-      <c r="X114" s="11"/>
-    </row>
-    <row r="115" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U115" s="11"/>
-      <c r="X115" s="11"/>
-    </row>
-    <row r="116" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U116" s="11"/>
-      <c r="X116" s="11"/>
-    </row>
-    <row r="117" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U117" s="11"/>
-      <c r="X117" s="11"/>
-    </row>
-    <row r="118" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U118" s="11"/>
-      <c r="X118" s="11"/>
-    </row>
-    <row r="119" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U119" s="11"/>
-      <c r="X119" s="11"/>
-    </row>
-    <row r="120" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U120" s="11"/>
-      <c r="X120" s="11"/>
-    </row>
-    <row r="121" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U121" s="11"/>
-      <c r="X121" s="11"/>
-    </row>
-    <row r="122" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U122" s="11"/>
-      <c r="X122" s="11"/>
-    </row>
-    <row r="123" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U123" s="11"/>
-      <c r="X123" s="11"/>
-    </row>
-    <row r="124" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U124" s="11"/>
-      <c r="X124" s="11"/>
-    </row>
-    <row r="125" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U125" s="11"/>
-      <c r="X125" s="11"/>
-    </row>
-    <row r="126" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U126" s="11"/>
-      <c r="X126" s="11"/>
-    </row>
-    <row r="127" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U127" s="11"/>
-      <c r="X127" s="11"/>
-    </row>
-    <row r="128" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U128" s="11"/>
-      <c r="X128" s="11"/>
-    </row>
-    <row r="129" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U129" s="11"/>
-      <c r="X129" s="11"/>
-    </row>
-    <row r="130" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U130" s="11"/>
-      <c r="X130" s="11"/>
-    </row>
-    <row r="131" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U131" s="11"/>
-      <c r="X131" s="11"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:Y136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6905,7 +6044,7 @@
     </row>
     <row r="3" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>9</v>
@@ -6934,19 +6073,19 @@
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
       <c r="R3" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="S3" s="25" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="T3" s="8"/>
       <c r="U3" s="24"/>
       <c r="V3" s="8"/>
       <c r="W3" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="X3" s="34" t="s">
-        <v>72</v>
+        <v>67</v>
+      </c>
+      <c r="X3" s="25" t="s">
+        <v>68</v>
       </c>
       <c r="Y3" s="8" t="s">
         <v>0</v>
@@ -6990,7 +6129,7 @@
         <v>0</v>
       </c>
       <c r="W4" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="X4" s="18" t="s">
         <v>11</v>
@@ -7055,7 +6194,7 @@
       <c r="B6" s="5"/>
       <c r="C6" s="9"/>
       <c r="D6" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -7063,29 +6202,24 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="R6" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="S6" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="T6" s="17"/>
-      <c r="U6" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="W6" t="s">
-        <v>75</v>
-      </c>
-      <c r="X6" s="33" t="s">
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="V6" s="5"/>
+      <c r="W6" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="X6" s="35" t="s">
         <v>17</v>
       </c>
       <c r="Y6" s="5"/>
@@ -7094,9 +6228,7 @@
       <c r="A7" s="6"/>
       <c r="B7" s="5"/>
       <c r="C7" s="9"/>
-      <c r="D7" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
         <v>13</v>
       </c>
@@ -7105,159 +6237,1259 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
       <c r="R7" s="17"/>
-      <c r="S7" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="T7" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="U7" s="33">
+      <c r="S7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="T7" s="5"/>
+      <c r="U7" s="18">
         <v>1</v>
       </c>
-      <c r="V7" s="9" t="s">
+      <c r="V7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="W7" s="35" t="s">
-        <v>0</v>
-      </c>
+      <c r="W7" s="19"/>
+      <c r="X7" s="20"/>
       <c r="Y7" s="5"/>
     </row>
     <row r="8" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="5"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="R8" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="S8" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="T8" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="U8" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="V8" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="W8" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="X8" s="33" t="s">
-        <v>0</v>
-      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="T8" s="5"/>
+      <c r="U8" s="18">
+        <v>1</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="W8" s="19"/>
+      <c r="X8" s="20"/>
       <c r="Y8" s="5"/>
     </row>
-    <row r="9" spans="1:25" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="5" t="s">
+    <row r="9" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="T9" s="5"/>
+      <c r="U9" s="18">
+        <v>1</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="W9" s="19"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="5"/>
+    </row>
+    <row r="10" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="5"/>
+    </row>
+    <row r="11" spans="1:25" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="19"/>
+    </row>
+    <row r="12" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="S12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="T12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="U12" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="V12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="X12" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X13" s="11"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X14" s="11"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X15" s="11"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X16" s="11"/>
+    </row>
+    <row r="17" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="X17" s="11"/>
+    </row>
+    <row r="18" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="X18" s="11"/>
+    </row>
+    <row r="19" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="X19" s="11"/>
+    </row>
+    <row r="20" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="X20" s="11"/>
+    </row>
+    <row r="21" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="X21" s="11"/>
+    </row>
+    <row r="22" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U22" s="11"/>
+      <c r="X22" s="11"/>
+    </row>
+    <row r="23" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U23" s="11"/>
+      <c r="X23" s="11"/>
+    </row>
+    <row r="24" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U24" s="11"/>
+      <c r="X24" s="11"/>
+    </row>
+    <row r="25" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U25" s="11"/>
+      <c r="X25" s="11"/>
+    </row>
+    <row r="26" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U26" s="11"/>
+      <c r="X26" s="11"/>
+    </row>
+    <row r="27" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U27" s="11"/>
+      <c r="X27" s="11"/>
+    </row>
+    <row r="28" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U28" s="11"/>
+      <c r="X28" s="11"/>
+    </row>
+    <row r="29" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U29" s="11"/>
+      <c r="X29" s="11"/>
+    </row>
+    <row r="30" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U30" s="11"/>
+      <c r="X30" s="11"/>
+    </row>
+    <row r="31" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U31" s="11"/>
+      <c r="X31" s="11"/>
+    </row>
+    <row r="32" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U32" s="11"/>
+      <c r="X32" s="11"/>
+    </row>
+    <row r="33" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U33" s="11"/>
+      <c r="X33" s="11"/>
+    </row>
+    <row r="34" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U34" s="11"/>
+      <c r="X34" s="11"/>
+    </row>
+    <row r="35" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U35" s="11"/>
+      <c r="X35" s="11"/>
+    </row>
+    <row r="36" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U36" s="11"/>
+      <c r="X36" s="11"/>
+    </row>
+    <row r="37" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U37" s="11"/>
+      <c r="X37" s="11"/>
+    </row>
+    <row r="38" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U38" s="11"/>
+      <c r="X38" s="11"/>
+    </row>
+    <row r="39" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U39" s="11"/>
+      <c r="X39" s="11"/>
+    </row>
+    <row r="40" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U40" s="11"/>
+      <c r="X40" s="11"/>
+    </row>
+    <row r="41" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U41" s="11"/>
+      <c r="X41" s="11"/>
+    </row>
+    <row r="42" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U42" s="11"/>
+      <c r="X42" s="11"/>
+    </row>
+    <row r="43" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U43" s="11"/>
+      <c r="X43" s="11"/>
+    </row>
+    <row r="44" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U44" s="11"/>
+      <c r="X44" s="11"/>
+    </row>
+    <row r="45" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U45" s="11"/>
+      <c r="X45" s="11"/>
+    </row>
+    <row r="46" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U46" s="11"/>
+      <c r="X46" s="11"/>
+    </row>
+    <row r="47" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U47" s="11"/>
+      <c r="X47" s="11"/>
+    </row>
+    <row r="48" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U48" s="11"/>
+      <c r="X48" s="11"/>
+    </row>
+    <row r="49" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U49" s="11"/>
+      <c r="X49" s="11"/>
+    </row>
+    <row r="50" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U50" s="11"/>
+      <c r="X50" s="11"/>
+    </row>
+    <row r="51" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U51" s="11"/>
+      <c r="X51" s="11"/>
+    </row>
+    <row r="52" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U52" s="11"/>
+      <c r="X52" s="11"/>
+    </row>
+    <row r="53" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U53" s="11"/>
+      <c r="X53" s="11"/>
+    </row>
+    <row r="54" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U54" s="11"/>
+      <c r="X54" s="11"/>
+    </row>
+    <row r="55" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U55" s="11"/>
+      <c r="X55" s="11"/>
+    </row>
+    <row r="56" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U56" s="11"/>
+      <c r="X56" s="11"/>
+    </row>
+    <row r="57" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U57" s="11"/>
+      <c r="X57" s="11"/>
+    </row>
+    <row r="58" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U58" s="11"/>
+      <c r="X58" s="11"/>
+    </row>
+    <row r="59" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U59" s="11"/>
+      <c r="X59" s="11"/>
+    </row>
+    <row r="60" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U60" s="11"/>
+      <c r="X60" s="11"/>
+    </row>
+    <row r="61" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U61" s="11"/>
+      <c r="X61" s="11"/>
+    </row>
+    <row r="62" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U62" s="11"/>
+      <c r="X62" s="11"/>
+    </row>
+    <row r="63" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U63" s="11"/>
+      <c r="X63" s="11"/>
+    </row>
+    <row r="64" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U64" s="11"/>
+      <c r="X64" s="11"/>
+    </row>
+    <row r="65" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U65" s="11"/>
+      <c r="X65" s="11"/>
+    </row>
+    <row r="66" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U66" s="11"/>
+      <c r="X66" s="11"/>
+    </row>
+    <row r="67" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U67" s="11"/>
+      <c r="X67" s="11"/>
+    </row>
+    <row r="68" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U68" s="11"/>
+      <c r="X68" s="11"/>
+    </row>
+    <row r="69" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U69" s="11"/>
+      <c r="X69" s="11"/>
+    </row>
+    <row r="70" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U70" s="11"/>
+      <c r="X70" s="11"/>
+    </row>
+    <row r="71" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U71" s="11"/>
+      <c r="X71" s="11"/>
+    </row>
+    <row r="72" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U72" s="11"/>
+      <c r="X72" s="11"/>
+    </row>
+    <row r="73" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U73" s="11"/>
+      <c r="X73" s="11"/>
+    </row>
+    <row r="74" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U74" s="11"/>
+      <c r="X74" s="11"/>
+    </row>
+    <row r="75" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U75" s="11"/>
+      <c r="X75" s="11"/>
+    </row>
+    <row r="76" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U76" s="11"/>
+      <c r="X76" s="11"/>
+    </row>
+    <row r="77" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U77" s="11"/>
+      <c r="X77" s="11"/>
+    </row>
+    <row r="78" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U78" s="11"/>
+      <c r="X78" s="11"/>
+    </row>
+    <row r="79" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U79" s="11"/>
+      <c r="X79" s="11"/>
+    </row>
+    <row r="80" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U80" s="11"/>
+      <c r="X80" s="11"/>
+    </row>
+    <row r="81" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U81" s="11"/>
+      <c r="X81" s="11"/>
+    </row>
+    <row r="82" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U82" s="11"/>
+      <c r="X82" s="11"/>
+    </row>
+    <row r="83" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U83" s="11"/>
+      <c r="X83" s="11"/>
+    </row>
+    <row r="84" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U84" s="11"/>
+      <c r="X84" s="11"/>
+    </row>
+    <row r="85" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U85" s="11"/>
+      <c r="X85" s="11"/>
+    </row>
+    <row r="86" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U86" s="11"/>
+      <c r="X86" s="11"/>
+    </row>
+    <row r="87" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U87" s="11"/>
+      <c r="X87" s="11"/>
+    </row>
+    <row r="88" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U88" s="11"/>
+      <c r="X88" s="11"/>
+    </row>
+    <row r="89" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U89" s="11"/>
+      <c r="X89" s="11"/>
+    </row>
+    <row r="90" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U90" s="11"/>
+      <c r="X90" s="11"/>
+    </row>
+    <row r="91" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U91" s="11"/>
+      <c r="X91" s="11"/>
+    </row>
+    <row r="92" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U92" s="11"/>
+      <c r="X92" s="11"/>
+    </row>
+    <row r="93" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U93" s="11"/>
+      <c r="X93" s="11"/>
+    </row>
+    <row r="94" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U94" s="11"/>
+      <c r="X94" s="11"/>
+    </row>
+    <row r="95" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U95" s="11"/>
+      <c r="X95" s="11"/>
+    </row>
+    <row r="96" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U96" s="11"/>
+      <c r="X96" s="11"/>
+    </row>
+    <row r="97" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U97" s="11"/>
+      <c r="X97" s="11"/>
+    </row>
+    <row r="98" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U98" s="11"/>
+      <c r="X98" s="11"/>
+    </row>
+    <row r="99" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U99" s="11"/>
+      <c r="X99" s="11"/>
+    </row>
+    <row r="100" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U100" s="11"/>
+      <c r="X100" s="11"/>
+    </row>
+    <row r="101" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U101" s="11"/>
+      <c r="X101" s="11"/>
+    </row>
+    <row r="102" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U102" s="11"/>
+      <c r="X102" s="11"/>
+    </row>
+    <row r="103" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U103" s="11"/>
+      <c r="X103" s="11"/>
+    </row>
+    <row r="104" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U104" s="11"/>
+      <c r="X104" s="11"/>
+    </row>
+    <row r="105" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U105" s="11"/>
+      <c r="X105" s="11"/>
+    </row>
+    <row r="106" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U106" s="11"/>
+      <c r="X106" s="11"/>
+    </row>
+    <row r="107" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U107" s="11"/>
+      <c r="X107" s="11"/>
+    </row>
+    <row r="108" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U108" s="11"/>
+      <c r="X108" s="11"/>
+    </row>
+    <row r="109" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U109" s="11"/>
+      <c r="X109" s="11"/>
+    </row>
+    <row r="110" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U110" s="11"/>
+      <c r="X110" s="11"/>
+    </row>
+    <row r="111" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U111" s="11"/>
+      <c r="X111" s="11"/>
+    </row>
+    <row r="112" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U112" s="11"/>
+      <c r="X112" s="11"/>
+    </row>
+    <row r="113" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U113" s="11"/>
+      <c r="X113" s="11"/>
+    </row>
+    <row r="114" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U114" s="11"/>
+      <c r="X114" s="11"/>
+    </row>
+    <row r="115" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U115" s="11"/>
+      <c r="X115" s="11"/>
+    </row>
+    <row r="116" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U116" s="11"/>
+      <c r="X116" s="11"/>
+    </row>
+    <row r="117" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U117" s="11"/>
+      <c r="X117" s="11"/>
+    </row>
+    <row r="118" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U118" s="11"/>
+      <c r="X118" s="11"/>
+    </row>
+    <row r="119" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U119" s="11"/>
+      <c r="X119" s="11"/>
+    </row>
+    <row r="120" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U120" s="11"/>
+      <c r="X120" s="11"/>
+    </row>
+    <row r="121" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U121" s="11"/>
+      <c r="X121" s="11"/>
+    </row>
+    <row r="122" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U122" s="11"/>
+      <c r="X122" s="11"/>
+    </row>
+    <row r="123" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U123" s="11"/>
+      <c r="X123" s="11"/>
+    </row>
+    <row r="124" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U124" s="11"/>
+      <c r="X124" s="11"/>
+    </row>
+    <row r="125" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U125" s="11"/>
+      <c r="X125" s="11"/>
+    </row>
+    <row r="126" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U126" s="11"/>
+      <c r="X126" s="11"/>
+    </row>
+    <row r="127" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U127" s="11"/>
+      <c r="X127" s="11"/>
+    </row>
+    <row r="128" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U128" s="11"/>
+      <c r="X128" s="11"/>
+    </row>
+    <row r="129" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U129" s="11"/>
+      <c r="X129" s="11"/>
+    </row>
+    <row r="130" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U130" s="11"/>
+      <c r="X130" s="11"/>
+    </row>
+    <row r="131" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U131" s="11"/>
+      <c r="X131" s="11"/>
+    </row>
+    <row r="132" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U132" s="11"/>
+      <c r="X132" s="11"/>
+    </row>
+    <row r="133" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U133" s="11"/>
+      <c r="X133" s="11"/>
+    </row>
+    <row r="134" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U134" s="11"/>
+      <c r="X134" s="11"/>
+    </row>
+    <row r="135" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U135" s="11"/>
+      <c r="X135" s="11"/>
+    </row>
+    <row r="136" spans="21:24" x14ac:dyDescent="0.25">
+      <c r="U136" s="11"/>
+      <c r="X136" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:X12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="10" style="11" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="1.85546875" style="11" customWidth="1"/>
+    <col min="10" max="11" width="2.7109375" style="11" customWidth="1"/>
+    <col min="12" max="16" width="2.7109375" style="11" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="11" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="11" customWidth="1"/>
+    <col min="19" max="20" width="11.42578125" style="11"/>
+    <col min="21" max="21" width="11.42578125" style="16"/>
+    <col min="22" max="23" width="11.42578125" style="11"/>
+    <col min="24" max="24" width="11.42578125" style="16"/>
+    <col min="25" max="16384" width="11.42578125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3">
+        <v>7</v>
+      </c>
+      <c r="H1" s="4">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3">
+        <v>9</v>
+      </c>
+      <c r="J1" s="4">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3">
+        <v>11</v>
+      </c>
+      <c r="L1" s="4">
+        <v>12</v>
+      </c>
+      <c r="M1" s="3">
+        <v>13</v>
+      </c>
+      <c r="N1" s="4">
+        <v>14</v>
+      </c>
+      <c r="O1" s="3">
+        <v>15</v>
+      </c>
+      <c r="P1" s="4">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="3">
+        <v>17</v>
+      </c>
+      <c r="R1" s="4">
+        <v>18</v>
+      </c>
+      <c r="S1" s="3">
+        <v>19</v>
+      </c>
+      <c r="T1" s="4">
+        <v>20</v>
+      </c>
+      <c r="U1" s="13">
+        <v>21</v>
+      </c>
+      <c r="V1" s="4">
+        <v>22</v>
+      </c>
+      <c r="W1" s="3">
+        <v>23</v>
+      </c>
+      <c r="X1" s="14">
+        <v>24</v>
+      </c>
+      <c r="Y1" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>63</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="S3" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="T3" s="8"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="X3" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y3" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4" s="18">
+        <v>1</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="W4" t="s">
+        <v>55</v>
+      </c>
+      <c r="X4" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="U5" s="18">
+        <v>1</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="W5" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="X5" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="V6" s="5"/>
+      <c r="W6" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="X6" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y6" s="5"/>
+    </row>
+    <row r="7" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="T7" s="5"/>
+      <c r="U7" s="18">
+        <v>1</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="W7" s="19"/>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="5"/>
+    </row>
+    <row r="8" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="T8" s="5"/>
+      <c r="U8" s="18">
+        <v>1</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="W8" s="19"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="5"/>
+    </row>
+    <row r="9" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="T9" s="5"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="19"/>
-    </row>
-    <row r="10" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="U9" s="18">
+        <v>1</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="W9" s="19"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="5"/>
+    </row>
+    <row r="10" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="5"/>
+    </row>
+    <row r="11" spans="1:25" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="19"/>
+    </row>
+    <row r="12" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="S10" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="T10" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="U10" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="V10" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="W10" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="X10" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="8" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="S12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="T12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="U12" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="V12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="X12" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="8" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>